<commit_message>
binary instead of tertiary system
</commit_message>
<xml_diff>
--- a/examples/full/flowsheet_data.xlsx
+++ b/examples/full/flowsheet_data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="48">
   <si>
     <t>flowsheet_data</t>
   </si>
@@ -22,13 +22,10 @@
     <t>stream_name</t>
   </si>
   <si>
-    <t>component_1_flowrate</t>
-  </si>
-  <si>
-    <t>component_2_flowrate</t>
-  </si>
-  <si>
-    <t>component_3_flowrate</t>
+    <t>component_A_flowrate</t>
+  </si>
+  <si>
+    <t>component_B_flowrate</t>
   </si>
   <si>
     <t>temperature</t>
@@ -58,7 +55,7 @@
     <t>DISTILLATION_COL</t>
   </si>
   <si>
-    <t>Raw feed to distillation column</t>
+    <t>Raw binary feed to distillation column</t>
   </si>
   <si>
     <t>S2</t>
@@ -70,7 +67,7 @@
     <t>CONDENSER</t>
   </si>
   <si>
-    <t>Top product from column</t>
+    <t>Top product from column (A-rich)</t>
   </si>
   <si>
     <t>S3</t>
@@ -82,7 +79,7 @@
     <t>REBOILER</t>
   </si>
   <si>
-    <t>Bottom product from column</t>
+    <t>Bottom product from column (B-rich)</t>
   </si>
   <si>
     <t>S4</t>
@@ -97,43 +94,43 @@
     <t>S5</t>
   </si>
   <si>
-    <t>Condensate</t>
+    <t>Net Distillate</t>
   </si>
   <si>
     <t>PRODUCT_TANK_1</t>
   </si>
   <si>
-    <t>Final distillate product</t>
+    <t>Final distillate product (A-rich)</t>
   </si>
   <si>
     <t>S6</t>
   </si>
   <si>
-    <t>Vapor to Reboiler</t>
+    <t>Reboiler Vapor</t>
+  </si>
+  <si>
+    <t>Vapor back to column</t>
+  </si>
+  <si>
+    <t>S7</t>
+  </si>
+  <si>
+    <t>Final Bottoms</t>
+  </si>
+  <si>
+    <t>PRODUCT_TANK_2</t>
+  </si>
+  <si>
+    <t>Final bottom product (B-rich)</t>
+  </si>
+  <si>
+    <t>S8</t>
+  </si>
+  <si>
+    <t>Steam</t>
   </si>
   <si>
     <t>STEAM_GENERATOR</t>
-  </si>
-  <si>
-    <t>Vapor for heating</t>
-  </si>
-  <si>
-    <t>S7</t>
-  </si>
-  <si>
-    <t>Final Bottoms</t>
-  </si>
-  <si>
-    <t>PRODUCT_TANK_2</t>
-  </si>
-  <si>
-    <t>Final bottom product</t>
-  </si>
-  <si>
-    <t>S8</t>
-  </si>
-  <si>
-    <t>Steam</t>
   </si>
   <si>
     <t>Heating steam</t>
@@ -1443,7 +1440,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:J12"/>
+  <dimension ref="A2:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1451,12 +1448,13 @@
   <cols>
     <col min="1" max="1" width="9.35156" style="1" customWidth="1"/>
     <col min="2" max="2" width="15.1719" style="1" customWidth="1"/>
-    <col min="3" max="5" width="19.6719" style="1" customWidth="1"/>
-    <col min="6" max="6" width="11.3516" style="1" customWidth="1"/>
-    <col min="7" max="7" width="8.5" style="1" customWidth="1"/>
-    <col min="8" max="9" width="17.8516" style="1" customWidth="1"/>
-    <col min="10" max="10" width="24.3516" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.35156" style="1" customWidth="1"/>
+    <col min="3" max="4" width="19.8516" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.3516" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.8516" style="1" customWidth="1"/>
+    <col min="8" max="8" width="16.3516" style="1" customWidth="1"/>
+    <col min="9" max="9" width="29.3516" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.35156" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="27.65" customHeight="1">
@@ -1471,7 +1469,6 @@
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
     </row>
     <row r="2" ht="20.25" customHeight="1">
       <c r="A2" t="s" s="3">
@@ -1501,240 +1498,216 @@
       <c r="I2" t="s" s="3">
         <v>9</v>
       </c>
-      <c r="J2" t="s" s="3">
-        <v>10</v>
-      </c>
     </row>
     <row r="3" ht="20.25" customHeight="1">
       <c r="A3" t="s" s="4">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s" s="5">
         <v>11</v>
-      </c>
-      <c r="B3" t="s" s="5">
-        <v>12</v>
       </c>
       <c r="C3" s="6">
         <v>100</v>
       </c>
       <c r="D3" s="6">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="E3" s="6">
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="F3" s="6">
-        <v>80</v>
-      </c>
-      <c r="G3" s="6">
         <v>1.5</v>
+      </c>
+      <c r="G3" t="s" s="7">
+        <v>12</v>
       </c>
       <c r="H3" t="s" s="7">
         <v>13</v>
       </c>
       <c r="I3" t="s" s="7">
         <v>14</v>
-      </c>
-      <c r="J3" t="s" s="7">
-        <v>15</v>
       </c>
     </row>
     <row r="4" ht="20.05" customHeight="1">
       <c r="A4" t="s" s="8">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s" s="9">
         <v>16</v>
       </c>
-      <c r="B4" t="s" s="9">
+      <c r="C4" s="10">
+        <v>95</v>
+      </c>
+      <c r="D4" s="10">
+        <v>2</v>
+      </c>
+      <c r="E4" s="10">
+        <v>65</v>
+      </c>
+      <c r="F4" s="10">
+        <v>1.2</v>
+      </c>
+      <c r="G4" t="s" s="11">
+        <v>13</v>
+      </c>
+      <c r="H4" t="s" s="11">
         <v>17</v>
-      </c>
-      <c r="C4" s="10">
-        <v>85</v>
-      </c>
-      <c r="D4" s="10">
-        <v>5</v>
-      </c>
-      <c r="E4" s="10">
-        <v>0.5</v>
-      </c>
-      <c r="F4" s="10">
-        <v>65</v>
-      </c>
-      <c r="G4" s="10">
-        <v>1.2</v>
-      </c>
-      <c r="H4" t="s" s="11">
-        <v>14</v>
       </c>
       <c r="I4" t="s" s="11">
         <v>18</v>
-      </c>
-      <c r="J4" t="s" s="11">
-        <v>19</v>
       </c>
     </row>
     <row r="5" ht="20.05" customHeight="1">
       <c r="A5" t="s" s="8">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s" s="9">
         <v>20</v>
       </c>
-      <c r="B5" t="s" s="9">
+      <c r="C5" s="10">
+        <v>5</v>
+      </c>
+      <c r="D5" s="10">
+        <v>58</v>
+      </c>
+      <c r="E5" s="10">
+        <v>120</v>
+      </c>
+      <c r="F5" s="10">
+        <v>1.6</v>
+      </c>
+      <c r="G5" t="s" s="11">
+        <v>13</v>
+      </c>
+      <c r="H5" t="s" s="11">
         <v>21</v>
-      </c>
-      <c r="C5" s="10">
-        <v>15</v>
-      </c>
-      <c r="D5" s="10">
-        <v>45</v>
-      </c>
-      <c r="E5" s="10">
-        <v>9.5</v>
-      </c>
-      <c r="F5" s="10">
-        <v>120</v>
-      </c>
-      <c r="G5" s="10">
-        <v>1.6</v>
-      </c>
-      <c r="H5" t="s" s="11">
-        <v>14</v>
       </c>
       <c r="I5" t="s" s="11">
         <v>22</v>
-      </c>
-      <c r="J5" t="s" s="11">
-        <v>23</v>
       </c>
     </row>
     <row r="6" ht="20.05" customHeight="1">
       <c r="A6" t="s" s="8">
+        <v>23</v>
+      </c>
+      <c r="B6" t="s" s="9">
         <v>24</v>
       </c>
-      <c r="B6" t="s" s="9">
+      <c r="C6" s="10">
+        <v>47.5</v>
+      </c>
+      <c r="D6" s="10">
+        <v>1</v>
+      </c>
+      <c r="E6" s="10">
+        <v>40</v>
+      </c>
+      <c r="F6" s="10">
+        <v>1.2</v>
+      </c>
+      <c r="G6" t="s" s="11">
+        <v>17</v>
+      </c>
+      <c r="H6" t="s" s="11">
+        <v>13</v>
+      </c>
+      <c r="I6" t="s" s="11">
         <v>25</v>
-      </c>
-      <c r="C6" s="10">
-        <v>42.5</v>
-      </c>
-      <c r="D6" s="10">
-        <v>2.5</v>
-      </c>
-      <c r="E6" s="10">
-        <v>0.25</v>
-      </c>
-      <c r="F6" s="10">
-        <v>35</v>
-      </c>
-      <c r="G6" s="10">
-        <v>1.2</v>
-      </c>
-      <c r="H6" t="s" s="11">
-        <v>18</v>
-      </c>
-      <c r="I6" t="s" s="11">
-        <v>14</v>
-      </c>
-      <c r="J6" t="s" s="11">
-        <v>26</v>
       </c>
     </row>
     <row r="7" ht="20.05" customHeight="1">
       <c r="A7" t="s" s="8">
+        <v>26</v>
+      </c>
+      <c r="B7" t="s" s="9">
         <v>27</v>
       </c>
-      <c r="B7" t="s" s="9">
+      <c r="C7" s="10">
+        <v>47.5</v>
+      </c>
+      <c r="D7" s="10">
+        <v>1</v>
+      </c>
+      <c r="E7" s="10">
+        <v>40</v>
+      </c>
+      <c r="F7" s="10">
+        <v>1.2</v>
+      </c>
+      <c r="G7" t="s" s="11">
+        <v>17</v>
+      </c>
+      <c r="H7" t="s" s="11">
         <v>28</v>
-      </c>
-      <c r="C7" s="10">
-        <v>42.5</v>
-      </c>
-      <c r="D7" s="10">
-        <v>2.5</v>
-      </c>
-      <c r="E7" s="10">
-        <v>0.25</v>
-      </c>
-      <c r="F7" s="10">
-        <v>35</v>
-      </c>
-      <c r="G7" s="10">
-        <v>1.2</v>
-      </c>
-      <c r="H7" t="s" s="11">
-        <v>18</v>
       </c>
       <c r="I7" t="s" s="11">
         <v>29</v>
-      </c>
-      <c r="J7" t="s" s="11">
-        <v>30</v>
       </c>
     </row>
     <row r="8" ht="20.05" customHeight="1">
       <c r="A8" t="s" s="8">
+        <v>30</v>
+      </c>
+      <c r="B8" t="s" s="9">
         <v>31</v>
       </c>
-      <c r="B8" t="s" s="9">
+      <c r="C8" s="10">
+        <v>5</v>
+      </c>
+      <c r="D8" s="10">
+        <v>58</v>
+      </c>
+      <c r="E8" s="10">
+        <v>120</v>
+      </c>
+      <c r="F8" s="10">
+        <v>1.6</v>
+      </c>
+      <c r="G8" t="s" s="11">
+        <v>21</v>
+      </c>
+      <c r="H8" t="s" s="11">
+        <v>13</v>
+      </c>
+      <c r="I8" t="s" s="11">
         <v>32</v>
-      </c>
-      <c r="C8" s="10">
-        <v>15</v>
-      </c>
-      <c r="D8" s="10">
-        <v>45</v>
-      </c>
-      <c r="E8" s="10">
-        <v>9.5</v>
-      </c>
-      <c r="F8" s="10">
-        <v>120</v>
-      </c>
-      <c r="G8" s="10">
-        <v>1.6</v>
-      </c>
-      <c r="H8" t="s" s="11">
-        <v>22</v>
-      </c>
-      <c r="I8" t="s" s="11">
-        <v>33</v>
-      </c>
-      <c r="J8" t="s" s="11">
-        <v>34</v>
       </c>
     </row>
     <row r="9" ht="20.05" customHeight="1">
       <c r="A9" t="s" s="8">
+        <v>33</v>
+      </c>
+      <c r="B9" t="s" s="9">
+        <v>34</v>
+      </c>
+      <c r="C9" s="10">
+        <v>5</v>
+      </c>
+      <c r="D9" s="10">
+        <v>58</v>
+      </c>
+      <c r="E9" s="10">
+        <v>110</v>
+      </c>
+      <c r="F9" s="10">
+        <v>1.4</v>
+      </c>
+      <c r="G9" t="s" s="11">
+        <v>21</v>
+      </c>
+      <c r="H9" t="s" s="11">
         <v>35</v>
       </c>
-      <c r="B9" t="s" s="9">
+      <c r="I9" t="s" s="11">
         <v>36</v>
-      </c>
-      <c r="C9" s="10">
-        <v>15</v>
-      </c>
-      <c r="D9" s="10">
-        <v>45</v>
-      </c>
-      <c r="E9" s="10">
-        <v>9.5</v>
-      </c>
-      <c r="F9" s="10">
-        <v>95</v>
-      </c>
-      <c r="G9" s="10">
-        <v>1.4</v>
-      </c>
-      <c r="H9" t="s" s="11">
-        <v>22</v>
-      </c>
-      <c r="I9" t="s" s="11">
-        <v>37</v>
-      </c>
-      <c r="J9" t="s" s="11">
-        <v>38</v>
       </c>
     </row>
     <row r="10" ht="20.05" customHeight="1">
       <c r="A10" t="s" s="8">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B10" t="s" s="9">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C10" s="10">
         <v>0</v>
@@ -1743,30 +1716,27 @@
         <v>0</v>
       </c>
       <c r="E10" s="10">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="F10" s="10">
-        <v>150</v>
-      </c>
-      <c r="G10" s="10">
         <v>3</v>
       </c>
+      <c r="G10" t="s" s="11">
+        <v>39</v>
+      </c>
       <c r="H10" t="s" s="11">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="I10" t="s" s="11">
-        <v>22</v>
-      </c>
-      <c r="J10" t="s" s="11">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" ht="20.05" customHeight="1">
       <c r="A11" t="s" s="8">
+        <v>41</v>
+      </c>
+      <c r="B11" t="s" s="9">
         <v>42</v>
-      </c>
-      <c r="B11" t="s" s="9">
-        <v>43</v>
       </c>
       <c r="C11" s="10">
         <v>0</v>
@@ -1775,30 +1745,27 @@
         <v>0</v>
       </c>
       <c r="E11" s="10">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="F11" s="10">
-        <v>25</v>
-      </c>
-      <c r="G11" s="10">
         <v>2</v>
       </c>
+      <c r="G11" t="s" s="11">
+        <v>43</v>
+      </c>
       <c r="H11" t="s" s="11">
+        <v>17</v>
+      </c>
+      <c r="I11" t="s" s="11">
         <v>44</v>
-      </c>
-      <c r="I11" t="s" s="11">
-        <v>18</v>
-      </c>
-      <c r="J11" t="s" s="11">
-        <v>45</v>
       </c>
     </row>
     <row r="12" ht="20.05" customHeight="1">
       <c r="A12" t="s" s="8">
+        <v>45</v>
+      </c>
+      <c r="B12" t="s" s="9">
         <v>46</v>
-      </c>
-      <c r="B12" t="s" s="9">
-        <v>47</v>
       </c>
       <c r="C12" s="10">
         <v>0</v>
@@ -1807,27 +1774,24 @@
         <v>0</v>
       </c>
       <c r="E12" s="10">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="F12" s="10">
-        <v>40</v>
-      </c>
-      <c r="G12" s="10">
         <v>1.8</v>
       </c>
+      <c r="G12" t="s" s="11">
+        <v>17</v>
+      </c>
       <c r="H12" t="s" s="11">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="I12" t="s" s="11">
-        <v>44</v>
-      </c>
-      <c r="J12" t="s" s="11">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A1:I1"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>